<commit_message>
fix for trade link attrs
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Attrs.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Attrs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>region2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>pset_pn</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>cset_cn</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>commodity</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>commodity2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>attribute</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>value</t>
         </is>
@@ -463,20 +473,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>SOUTH</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>TB_ELC_*,TU_ELC_*</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>ELC</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ELC</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>IRE_FLO</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>0.97</v>
       </c>
     </row>
@@ -488,20 +508,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>NORTH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>TB_ELC_*,TU_ELC_*</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>ELC</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ELC</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>IRE_FLO</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>0.97</v>
       </c>
     </row>

</xml_diff>